<commit_message>
added recipes and updated requirements
</commit_message>
<xml_diff>
--- a/src/recipes.xlsx
+++ b/src/recipes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krose\Repositories\opskrifter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krose\Desktop\Madplanlaegger\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB2E316-32F7-4958-9FF4-D127CB5A0B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA309F7-4FA1-442E-8693-379B35F6F028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{1DF9BAFE-AC5C-E845-B4CA-1FB82D7DF7D2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{1DF9BAFE-AC5C-E845-B4CA-1FB82D7DF7D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Retter" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="79">
   <si>
     <t>ID</t>
   </si>
@@ -156,6 +156,123 @@
   </si>
   <si>
     <t>Mayonaise</t>
+  </si>
+  <si>
+    <t>Sur-Sød Kylling</t>
+  </si>
+  <si>
+    <t>Kyllingebuillion</t>
+  </si>
+  <si>
+    <t>Peberfrugt</t>
+  </si>
+  <si>
+    <t>Ananas</t>
+  </si>
+  <si>
+    <t>Cashewnødder</t>
+  </si>
+  <si>
+    <t>Hoisinsauce</t>
+  </si>
+  <si>
+    <t>Hvidvinseddike</t>
+  </si>
+  <si>
+    <t>Sukker</t>
+  </si>
+  <si>
+    <t>tsk</t>
+  </si>
+  <si>
+    <t>Kokoskarry</t>
+  </si>
+  <si>
+    <t>Grøntsagsbuillion</t>
+  </si>
+  <si>
+    <t>Ris</t>
+  </si>
+  <si>
+    <t>Løg</t>
+  </si>
+  <si>
+    <t>Ingefær</t>
+  </si>
+  <si>
+    <t>Grønne linser</t>
+  </si>
+  <si>
+    <t>Karry</t>
+  </si>
+  <si>
+    <t>Gul Karrypasta</t>
+  </si>
+  <si>
+    <t>Kokosmælk</t>
+  </si>
+  <si>
+    <t>Koriander</t>
+  </si>
+  <si>
+    <t>Yoghurt</t>
+  </si>
+  <si>
+    <t>pakke</t>
+  </si>
+  <si>
+    <t>Kikærtekarry</t>
+  </si>
+  <si>
+    <t>Squash</t>
+  </si>
+  <si>
+    <t>Kikærter</t>
+  </si>
+  <si>
+    <t>Goan xacut</t>
+  </si>
+  <si>
+    <t>Abrikoschutney</t>
+  </si>
+  <si>
+    <t>Asiatisk inspireret kyllingewok</t>
+  </si>
+  <si>
+    <t>Lime</t>
+  </si>
+  <si>
+    <t>Nudler</t>
+  </si>
+  <si>
+    <t>Honning</t>
+  </si>
+  <si>
+    <t>Olivenolie</t>
+  </si>
+  <si>
+    <t>Peanuts</t>
+  </si>
+  <si>
+    <t>akke</t>
+  </si>
+  <si>
+    <t>psk</t>
+  </si>
+  <si>
+    <t>BBQ-marineret kylling</t>
+  </si>
+  <si>
+    <t>Bulgur</t>
+  </si>
+  <si>
+    <t>BBQ-sauce</t>
+  </si>
+  <si>
+    <t>Purløg</t>
+  </si>
+  <si>
+    <t>Appelsin</t>
   </si>
 </sst>
 </file>
@@ -191,8 +308,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,19 +625,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{788F640D-5B8E-BB42-BF76-8A0950424087}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -527,7 +645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -535,12 +653,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
       <c r="B3">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -550,15 +708,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1D6F3A-C42A-9249-9195-C7F544F55CEE}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -569,7 +727,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -580,7 +738,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -591,7 +749,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -602,7 +760,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -613,7 +771,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -624,7 +782,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -635,7 +793,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -646,7 +804,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -657,7 +815,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -668,7 +826,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -679,7 +837,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -690,7 +848,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -701,7 +859,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -712,7 +870,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -723,7 +881,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -734,7 +892,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -745,7 +903,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -756,7 +914,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -767,7 +925,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -778,7 +936,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -789,7 +947,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -800,7 +958,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -811,7 +969,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -822,7 +980,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -831,6 +989,336 @@
       </c>
       <c r="C25" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>67</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>69</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+      <c r="C50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>71</v>
+      </c>
+      <c r="B51">
+        <v>50</v>
+      </c>
+      <c r="C51" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52">
+        <v>51</v>
+      </c>
+      <c r="C52" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>76</v>
+      </c>
+      <c r="B53">
+        <v>52</v>
+      </c>
+      <c r="C53" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54">
+        <v>53</v>
+      </c>
+      <c r="C54" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>78</v>
+      </c>
+      <c r="B55">
+        <v>54</v>
+      </c>
+      <c r="C55" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -840,19 +1328,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46356CDD-C11E-954C-B72D-1CB56AB59220}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -875,7 +1363,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -901,7 +1389,7 @@
         <v>stk</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -927,7 +1415,7 @@
         <v>gram</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -953,7 +1441,7 @@
         <v>stk</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -979,7 +1467,7 @@
         <v>fed</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1005,7 +1493,7 @@
         <v>stk</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1031,7 +1519,7 @@
         <v>dl</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1057,7 +1545,7 @@
         <v>gram</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1083,7 +1571,7 @@
         <v>gram</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1109,7 +1597,7 @@
         <v>stk</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1135,7 +1623,7 @@
         <v>pose</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1161,7 +1649,7 @@
         <v>ml</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1187,7 +1675,7 @@
         <v>gram</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1213,7 +1701,7 @@
         <v>gram</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1239,7 +1727,7 @@
         <v>gram</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1265,7 +1753,7 @@
         <v>stk</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1291,7 +1779,7 @@
         <v>gram</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1317,7 +1805,7 @@
         <v>fed</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1343,7 +1831,7 @@
         <v>gram</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1369,7 +1857,7 @@
         <v>pose(r)</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1395,7 +1883,7 @@
         <v>stk</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1421,7 +1909,7 @@
         <v>stk</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1447,7 +1935,7 @@
         <v>stk</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1473,7 +1961,7 @@
         <v>gram</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1499,7 +1987,7 @@
         <v>ml</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1522,6 +2010,1581 @@
       </c>
       <c r="G26" t="str">
         <f>VLOOKUP(D26,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27">
+        <v>400</v>
+      </c>
+      <c r="F27">
+        <f>VLOOKUP(D27,Ingredienser!A:C,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="G27" t="str">
+        <f>VLOOKUP(D27,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <f>VLOOKUP(D28,Ingredienser!A:C,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="G28" t="str">
+        <f>VLOOKUP(D28,Ingredienser!A:C,3,FALSE)</f>
+        <v>fed</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <f>VLOOKUP(D29,Ingredienser!A:C,2,FALSE)</f>
+        <v>25</v>
+      </c>
+      <c r="G29" t="str">
+        <f>VLOOKUP(D29,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <f>VLOOKUP(D30,Ingredienser!A:C,2,FALSE)</f>
+        <v>26</v>
+      </c>
+      <c r="G30" t="str">
+        <f>VLOOKUP(D30,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31">
+        <v>50</v>
+      </c>
+      <c r="F31">
+        <f>VLOOKUP(D31,Ingredienser!A:C,2,FALSE)</f>
+        <v>27</v>
+      </c>
+      <c r="G31" t="str">
+        <f>VLOOKUP(D31,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <f>VLOOKUP(D32,Ingredienser!A:C,2,FALSE)</f>
+        <v>21</v>
+      </c>
+      <c r="G32" t="str">
+        <f>VLOOKUP(D32,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33">
+        <v>20</v>
+      </c>
+      <c r="F33">
+        <f>VLOOKUP(D33,Ingredienser!A:C,2,FALSE)</f>
+        <v>28</v>
+      </c>
+      <c r="G33" t="str">
+        <f>VLOOKUP(D33,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34">
+        <v>25</v>
+      </c>
+      <c r="F34">
+        <f>VLOOKUP(D34,Ingredienser!A:C,2,FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="G34" t="str">
+        <f>VLOOKUP(D34,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35" t="s">
+        <v>45</v>
+      </c>
+      <c r="E35">
+        <v>30</v>
+      </c>
+      <c r="F35">
+        <f>VLOOKUP(D35,Ingredienser!A:C,2,FALSE)</f>
+        <v>29</v>
+      </c>
+      <c r="G35" t="str">
+        <f>VLOOKUP(D35,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>46</v>
+      </c>
+      <c r="E36">
+        <v>25</v>
+      </c>
+      <c r="F36">
+        <f>VLOOKUP(D36,Ingredienser!A:C,2,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="G36" t="str">
+        <f>VLOOKUP(D36,Ingredienser!A:C,3,FALSE)</f>
+        <v>ml</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <f>VLOOKUP(D37,Ingredienser!A:C,2,FALSE)</f>
+        <v>31</v>
+      </c>
+      <c r="G37" t="str">
+        <f>VLOOKUP(D37,Ingredienser!A:C,3,FALSE)</f>
+        <v>tsk</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <f>VLOOKUP(D38,Ingredienser!A:C,2,FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="G38" t="str">
+        <f>VLOOKUP(D38,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39">
+        <v>100</v>
+      </c>
+      <c r="F39">
+        <f>VLOOKUP(D39,Ingredienser!A:C,2,FALSE)</f>
+        <v>33</v>
+      </c>
+      <c r="G39" t="str">
+        <f>VLOOKUP(D39,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40">
+        <f>VLOOKUP(D40,Ingredienser!A:C,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="G40" t="str">
+        <f>VLOOKUP(D40,Ingredienser!A:C,3,FALSE)</f>
+        <v>fed</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+      <c r="D41" t="s">
+        <v>52</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <f>VLOOKUP(D41,Ingredienser!A:C,2,FALSE)</f>
+        <v>34</v>
+      </c>
+      <c r="G41" t="str">
+        <f>VLOOKUP(D41,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>53</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <f>VLOOKUP(D42,Ingredienser!A:C,2,FALSE)</f>
+        <v>35</v>
+      </c>
+      <c r="G42" t="str">
+        <f>VLOOKUP(D42,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="D43" t="s">
+        <v>35</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <f>VLOOKUP(D43,Ingredienser!A:C,2,FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="G43" t="str">
+        <f>VLOOKUP(D43,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44">
+        <f>VLOOKUP(D44,Ingredienser!A:C,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="G44" t="str">
+        <f>VLOOKUP(D44,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="D45" t="s">
+        <v>54</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <f>VLOOKUP(D45,Ingredienser!A:C,2,FALSE)</f>
+        <v>36</v>
+      </c>
+      <c r="G45" t="str">
+        <f>VLOOKUP(D45,Ingredienser!A:C,3,FALSE)</f>
+        <v>pakke</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46" t="s">
+        <v>55</v>
+      </c>
+      <c r="E46">
+        <v>4</v>
+      </c>
+      <c r="F46">
+        <f>VLOOKUP(D46,Ingredienser!A:C,2,FALSE)</f>
+        <v>37</v>
+      </c>
+      <c r="G46" t="str">
+        <f>VLOOKUP(D46,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+      <c r="D47" t="s">
+        <v>56</v>
+      </c>
+      <c r="E47">
+        <v>20</v>
+      </c>
+      <c r="F47">
+        <f>VLOOKUP(D47,Ingredienser!A:C,2,FALSE)</f>
+        <v>38</v>
+      </c>
+      <c r="G47" t="str">
+        <f>VLOOKUP(D47,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48">
+        <v>4</v>
+      </c>
+      <c r="D48" t="s">
+        <v>57</v>
+      </c>
+      <c r="E48">
+        <v>200</v>
+      </c>
+      <c r="F48">
+        <f>VLOOKUP(D48,Ingredienser!A:C,2,FALSE)</f>
+        <v>39</v>
+      </c>
+      <c r="G48" t="str">
+        <f>VLOOKUP(D48,Ingredienser!A:C,3,FALSE)</f>
+        <v>ml</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
+      </c>
+      <c r="D49" t="s">
+        <v>38</v>
+      </c>
+      <c r="E49">
+        <v>25</v>
+      </c>
+      <c r="F49">
+        <f>VLOOKUP(D49,Ingredienser!A:C,2,FALSE)</f>
+        <v>23</v>
+      </c>
+      <c r="G49" t="str">
+        <f>VLOOKUP(D49,Ingredienser!A:C,3,FALSE)</f>
+        <v>ml</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>4</v>
+      </c>
+      <c r="D50" t="s">
+        <v>58</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <f>VLOOKUP(D50,Ingredienser!A:C,2,FALSE)</f>
+        <v>40</v>
+      </c>
+      <c r="G50" t="str">
+        <f>VLOOKUP(D50,Ingredienser!A:C,3,FALSE)</f>
+        <v>pose</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="D51" t="s">
+        <v>44</v>
+      </c>
+      <c r="E51">
+        <v>20</v>
+      </c>
+      <c r="F51">
+        <f>VLOOKUP(D51,Ingredienser!A:C,2,FALSE)</f>
+        <v>28</v>
+      </c>
+      <c r="G51" t="str">
+        <f>VLOOKUP(D51,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>49</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
+      </c>
+      <c r="D52" t="s">
+        <v>59</v>
+      </c>
+      <c r="E52">
+        <v>75</v>
+      </c>
+      <c r="F52">
+        <f>VLOOKUP(D52,Ingredienser!A:C,2,FALSE)</f>
+        <v>41</v>
+      </c>
+      <c r="G52" t="str">
+        <f>VLOOKUP(D52,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53">
+        <v>5</v>
+      </c>
+      <c r="D53" t="s">
+        <v>51</v>
+      </c>
+      <c r="E53">
+        <v>150</v>
+      </c>
+      <c r="F53">
+        <f>VLOOKUP(D53,Ingredienser!A:C,2,FALSE)</f>
+        <v>33</v>
+      </c>
+      <c r="G53" t="str">
+        <f>VLOOKUP(D53,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>61</v>
+      </c>
+      <c r="C54">
+        <v>5</v>
+      </c>
+      <c r="D54" t="s">
+        <v>26</v>
+      </c>
+      <c r="E54">
+        <v>5</v>
+      </c>
+      <c r="F54">
+        <f>VLOOKUP(D54,Ingredienser!A:C,2,FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="G54" t="str">
+        <f>VLOOKUP(D54,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55">
+        <v>5</v>
+      </c>
+      <c r="D55" t="s">
+        <v>53</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <f>VLOOKUP(D55,Ingredienser!A:C,2,FALSE)</f>
+        <v>35</v>
+      </c>
+      <c r="G55" t="str">
+        <f>VLOOKUP(D55,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56">
+        <v>5</v>
+      </c>
+      <c r="D56" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <f>VLOOKUP(D56,Ingredienser!A:C,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="G56" t="str">
+        <f>VLOOKUP(D56,Ingredienser!A:C,3,FALSE)</f>
+        <v>fed</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+      <c r="D57" t="s">
+        <v>62</v>
+      </c>
+      <c r="E57">
+        <v>0.5</v>
+      </c>
+      <c r="F57">
+        <f>VLOOKUP(D57,Ingredienser!A:C,2,FALSE)</f>
+        <v>42</v>
+      </c>
+      <c r="G57" t="str">
+        <f>VLOOKUP(D57,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>5</v>
+      </c>
+      <c r="D58" t="s">
+        <v>35</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <f>VLOOKUP(D58,Ingredienser!A:C,2,FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="G58" t="str">
+        <f>VLOOKUP(D58,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>61</v>
+      </c>
+      <c r="C59">
+        <v>5</v>
+      </c>
+      <c r="D59" t="s">
+        <v>14</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <f>VLOOKUP(D59,Ingredienser!A:C,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="G59" t="str">
+        <f>VLOOKUP(D59,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60">
+        <v>5</v>
+      </c>
+      <c r="D60" t="s">
+        <v>63</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <f>VLOOKUP(D60,Ingredienser!A:C,2,FALSE)</f>
+        <v>43</v>
+      </c>
+      <c r="G60" t="str">
+        <f>VLOOKUP(D60,Ingredienser!A:C,3,FALSE)</f>
+        <v>pakke</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>61</v>
+      </c>
+      <c r="C61">
+        <v>5</v>
+      </c>
+      <c r="D61" t="s">
+        <v>58</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <f>VLOOKUP(D61,Ingredienser!A:C,2,FALSE)</f>
+        <v>40</v>
+      </c>
+      <c r="G61" t="str">
+        <f>VLOOKUP(D61,Ingredienser!A:C,3,FALSE)</f>
+        <v>pose</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>61</v>
+      </c>
+      <c r="C62">
+        <v>5</v>
+      </c>
+      <c r="D62" t="s">
+        <v>56</v>
+      </c>
+      <c r="E62">
+        <v>20</v>
+      </c>
+      <c r="F62">
+        <f>VLOOKUP(D62,Ingredienser!A:C,2,FALSE)</f>
+        <v>38</v>
+      </c>
+      <c r="G62" t="str">
+        <f>VLOOKUP(D62,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>61</v>
+      </c>
+      <c r="C63">
+        <v>5</v>
+      </c>
+      <c r="D63" t="s">
+        <v>64</v>
+      </c>
+      <c r="E63">
+        <v>3</v>
+      </c>
+      <c r="F63">
+        <f>VLOOKUP(D63,Ingredienser!A:C,2,FALSE)</f>
+        <v>44</v>
+      </c>
+      <c r="G63" t="str">
+        <f>VLOOKUP(D63,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>61</v>
+      </c>
+      <c r="C64">
+        <v>5</v>
+      </c>
+      <c r="D64" t="s">
+        <v>57</v>
+      </c>
+      <c r="E64">
+        <v>250</v>
+      </c>
+      <c r="F64">
+        <f>VLOOKUP(D64,Ingredienser!A:C,2,FALSE)</f>
+        <v>39</v>
+      </c>
+      <c r="G64" t="str">
+        <f>VLOOKUP(D64,Ingredienser!A:C,3,FALSE)</f>
+        <v>ml</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>61</v>
+      </c>
+      <c r="C65">
+        <v>5</v>
+      </c>
+      <c r="D65" t="s">
+        <v>65</v>
+      </c>
+      <c r="E65">
+        <v>50</v>
+      </c>
+      <c r="F65">
+        <f>VLOOKUP(D65,Ingredienser!A:C,2,FALSE)</f>
+        <v>45</v>
+      </c>
+      <c r="G65" t="str">
+        <f>VLOOKUP(D65,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>66</v>
+      </c>
+      <c r="C66">
+        <v>6</v>
+      </c>
+      <c r="D66" t="s">
+        <v>53</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <f>VLOOKUP(D66,Ingredienser!A:C,2,FALSE)</f>
+        <v>35</v>
+      </c>
+      <c r="G66" t="str">
+        <f>VLOOKUP(D66,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>66</v>
+      </c>
+      <c r="C67">
+        <v>6</v>
+      </c>
+      <c r="D67" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67">
+        <v>4</v>
+      </c>
+      <c r="F67">
+        <f>VLOOKUP(D67,Ingredienser!A:C,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="G67" t="str">
+        <f>VLOOKUP(D67,Ingredienser!A:C,3,FALSE)</f>
+        <v>fed</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>66</v>
+      </c>
+      <c r="C68">
+        <v>6</v>
+      </c>
+      <c r="D68" t="s">
+        <v>36</v>
+      </c>
+      <c r="E68">
+        <v>4</v>
+      </c>
+      <c r="F68">
+        <f>VLOOKUP(D68,Ingredienser!A:C,2,FALSE)</f>
+        <v>21</v>
+      </c>
+      <c r="G68" t="str">
+        <f>VLOOKUP(D68,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>66</v>
+      </c>
+      <c r="C69">
+        <v>6</v>
+      </c>
+      <c r="D69" t="s">
+        <v>26</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69">
+        <f>VLOOKUP(D69,Ingredienser!A:C,2,FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="G69" t="str">
+        <f>VLOOKUP(D69,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>66</v>
+      </c>
+      <c r="C70">
+        <v>6</v>
+      </c>
+      <c r="D70" t="s">
+        <v>67</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <f>VLOOKUP(D70,Ingredienser!A:C,2,FALSE)</f>
+        <v>46</v>
+      </c>
+      <c r="G70" t="str">
+        <f>VLOOKUP(D70,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>66</v>
+      </c>
+      <c r="C71">
+        <v>6</v>
+      </c>
+      <c r="D71" t="s">
+        <v>35</v>
+      </c>
+      <c r="E71">
+        <v>2</v>
+      </c>
+      <c r="F71">
+        <f>VLOOKUP(D71,Ingredienser!A:C,2,FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="G71" t="str">
+        <f>VLOOKUP(D71,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>66</v>
+      </c>
+      <c r="C72">
+        <v>6</v>
+      </c>
+      <c r="D72" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72">
+        <v>2</v>
+      </c>
+      <c r="F72">
+        <f>VLOOKUP(D72,Ingredienser!A:C,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="G72" t="str">
+        <f>VLOOKUP(D72,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>66</v>
+      </c>
+      <c r="C73">
+        <v>6</v>
+      </c>
+      <c r="D73" t="s">
+        <v>68</v>
+      </c>
+      <c r="E73" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F73">
+        <f>VLOOKUP(D73,Ingredienser!A:C,2,FALSE)</f>
+        <v>47</v>
+      </c>
+      <c r="G73" t="str">
+        <f>VLOOKUP(D73,Ingredienser!A:C,3,FALSE)</f>
+        <v>pakke</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>66</v>
+      </c>
+      <c r="C74">
+        <v>6</v>
+      </c>
+      <c r="D74" t="s">
+        <v>38</v>
+      </c>
+      <c r="E74" s="1">
+        <v>20</v>
+      </c>
+      <c r="F74">
+        <f>VLOOKUP(D74,Ingredienser!A:C,2,FALSE)</f>
+        <v>23</v>
+      </c>
+      <c r="G74" t="str">
+        <f>VLOOKUP(D74,Ingredienser!A:C,3,FALSE)</f>
+        <v>ml</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>66</v>
+      </c>
+      <c r="C75">
+        <v>6</v>
+      </c>
+      <c r="D75" t="s">
+        <v>69</v>
+      </c>
+      <c r="E75" s="1">
+        <v>1</v>
+      </c>
+      <c r="F75">
+        <f>VLOOKUP(D75,Ingredienser!A:C,2,FALSE)</f>
+        <v>48</v>
+      </c>
+      <c r="G75" t="str">
+        <f>VLOOKUP(D75,Ingredienser!A:C,3,FALSE)</f>
+        <v>akke</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>66</v>
+      </c>
+      <c r="C76">
+        <v>6</v>
+      </c>
+      <c r="D76" t="s">
+        <v>70</v>
+      </c>
+      <c r="E76" s="1">
+        <v>2</v>
+      </c>
+      <c r="F76">
+        <f>VLOOKUP(D76,Ingredienser!A:C,2,FALSE)</f>
+        <v>49</v>
+      </c>
+      <c r="G76" t="str">
+        <f>VLOOKUP(D76,Ingredienser!A:C,3,FALSE)</f>
+        <v>psk</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>66</v>
+      </c>
+      <c r="C77">
+        <v>6</v>
+      </c>
+      <c r="D77" t="s">
+        <v>12</v>
+      </c>
+      <c r="E77" s="1">
+        <v>300</v>
+      </c>
+      <c r="F77">
+        <f>VLOOKUP(D77,Ingredienser!A:C,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="G77" t="str">
+        <f>VLOOKUP(D77,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>66</v>
+      </c>
+      <c r="C78">
+        <v>6</v>
+      </c>
+      <c r="D78" t="s">
+        <v>58</v>
+      </c>
+      <c r="E78" s="1">
+        <v>1</v>
+      </c>
+      <c r="F78">
+        <f>VLOOKUP(D78,Ingredienser!A:C,2,FALSE)</f>
+        <v>40</v>
+      </c>
+      <c r="G78" t="str">
+        <f>VLOOKUP(D78,Ingredienser!A:C,3,FALSE)</f>
+        <v>pose</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>66</v>
+      </c>
+      <c r="C79">
+        <v>6</v>
+      </c>
+      <c r="D79" t="s">
+        <v>71</v>
+      </c>
+      <c r="E79" s="1">
+        <v>40</v>
+      </c>
+      <c r="F79">
+        <f>VLOOKUP(D79,Ingredienser!A:C,2,FALSE)</f>
+        <v>50</v>
+      </c>
+      <c r="G79" t="str">
+        <f>VLOOKUP(D79,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>74</v>
+      </c>
+      <c r="C80">
+        <v>7</v>
+      </c>
+      <c r="D80" t="s">
+        <v>75</v>
+      </c>
+      <c r="E80" s="1">
+        <v>170</v>
+      </c>
+      <c r="F80">
+        <f>VLOOKUP(D80,Ingredienser!A:C,2,FALSE)</f>
+        <v>51</v>
+      </c>
+      <c r="G80" t="str">
+        <f>VLOOKUP(D80,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>74</v>
+      </c>
+      <c r="C81">
+        <v>7</v>
+      </c>
+      <c r="D81" t="s">
+        <v>41</v>
+      </c>
+      <c r="E81" s="1">
+        <v>8</v>
+      </c>
+      <c r="F81">
+        <f>VLOOKUP(D81,Ingredienser!A:C,2,FALSE)</f>
+        <v>25</v>
+      </c>
+      <c r="G81" t="str">
+        <f>VLOOKUP(D81,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>74</v>
+      </c>
+      <c r="C82">
+        <v>7</v>
+      </c>
+      <c r="D82" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" s="1">
+        <v>2</v>
+      </c>
+      <c r="F82">
+        <f>VLOOKUP(D82,Ingredienser!A:C,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="G82" t="str">
+        <f>VLOOKUP(D82,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>74</v>
+      </c>
+      <c r="C83">
+        <v>7</v>
+      </c>
+      <c r="D83" t="s">
+        <v>12</v>
+      </c>
+      <c r="E83" s="1">
+        <v>500</v>
+      </c>
+      <c r="F83">
+        <f>VLOOKUP(D83,Ingredienser!A:C,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="G83" t="str">
+        <f>VLOOKUP(D83,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>74</v>
+      </c>
+      <c r="C84">
+        <v>7</v>
+      </c>
+      <c r="D84" t="s">
+        <v>76</v>
+      </c>
+      <c r="E84" s="1">
+        <v>120</v>
+      </c>
+      <c r="F84">
+        <f>VLOOKUP(D84,Ingredienser!A:C,2,FALSE)</f>
+        <v>52</v>
+      </c>
+      <c r="G84" t="str">
+        <f>VLOOKUP(D84,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>74</v>
+      </c>
+      <c r="C85">
+        <v>7</v>
+      </c>
+      <c r="D85" t="s">
+        <v>14</v>
+      </c>
+      <c r="E85" s="1">
+        <v>2</v>
+      </c>
+      <c r="F85">
+        <f>VLOOKUP(D85,Ingredienser!A:C,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="G85" t="str">
+        <f>VLOOKUP(D85,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>74</v>
+      </c>
+      <c r="C86">
+        <v>7</v>
+      </c>
+      <c r="D86" t="s">
+        <v>10</v>
+      </c>
+      <c r="E86" s="1">
+        <v>1</v>
+      </c>
+      <c r="F86">
+        <f>VLOOKUP(D86,Ingredienser!A:C,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="G86" t="str">
+        <f>VLOOKUP(D86,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>74</v>
+      </c>
+      <c r="C87">
+        <v>7</v>
+      </c>
+      <c r="D87" t="s">
+        <v>77</v>
+      </c>
+      <c r="E87" s="1">
+        <v>1</v>
+      </c>
+      <c r="F87">
+        <f>VLOOKUP(D87,Ingredienser!A:C,2,FALSE)</f>
+        <v>53</v>
+      </c>
+      <c r="G87" t="str">
+        <f>VLOOKUP(D87,Ingredienser!A:C,3,FALSE)</f>
+        <v>pose</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>74</v>
+      </c>
+      <c r="C88">
+        <v>7</v>
+      </c>
+      <c r="D88" t="s">
+        <v>78</v>
+      </c>
+      <c r="E88" s="1">
+        <v>1</v>
+      </c>
+      <c r="F88">
+        <f>VLOOKUP(D88,Ingredienser!A:C,2,FALSE)</f>
+        <v>54</v>
+      </c>
+      <c r="G88" t="str">
+        <f>VLOOKUP(D88,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>74</v>
+      </c>
+      <c r="C89">
+        <v>7</v>
+      </c>
+      <c r="D89" t="s">
+        <v>27</v>
+      </c>
+      <c r="E89" s="1">
+        <v>80</v>
+      </c>
+      <c r="F89">
+        <f>VLOOKUP(D89,Ingredienser!A:C,2,FALSE)</f>
+        <v>13</v>
+      </c>
+      <c r="G89" t="str">
+        <f>VLOOKUP(D89,Ingredienser!A:C,3,FALSE)</f>
         <v>gram</v>
       </c>
     </row>

</xml_diff>